<commit_message>
Deployed 2457835 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA 12S metab/example_output/Breakdown_ASV_level.xlsx
+++ b/eDNA 12S metab/example_output/Breakdown_ASV_level.xlsx
@@ -4592,7 +4592,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>e097ec8e447187fdeadfe7705dc2c3ee</t>
+          <t>ba360a9c42a6558cd9d02ac7f13e0fa9</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -4622,7 +4622,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>ba360a9c42a6558cd9d02ac7f13e0fa9</t>
+          <t>e097ec8e447187fdeadfe7705dc2c3ee</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -4922,7 +4922,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>7a92f84ef422774b0a9c4387869d34d7</t>
+          <t>18f0ba977064dc968ac59ce7bb3baaa8</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -4952,7 +4952,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>18f0ba977064dc968ac59ce7bb3baaa8</t>
+          <t>7a92f84ef422774b0a9c4387869d34d7</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">

</xml_diff>